<commit_message>
removed snapshots, added more code for cleaning
</commit_message>
<xml_diff>
--- a/data/Data_Dictionary.xlsx
+++ b/data/Data_Dictionary.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siddh\Desktop\LendingClubCaseStudy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA1CB10-B0A2-4910-83BF-A8E2B27E62F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37A2A1-6356-4BB6-9464-B932997FEE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13245" yWindow="1650" windowWidth="23985" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12675" yWindow="330" windowWidth="23985" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId2"/>
-    <sheet name="RejectStats" sheetId="7" r:id="rId3"/>
+    <sheet name="RejectStats" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$K$116</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$J$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RejectStats!$A$1:$B$10</definedName>
     <definedName name="behav">#REF!</definedName>
     <definedName name="data_dict">LoanStats!$A$1:$B$116</definedName>
-    <definedName name="dropped">Sheet2!$A$3:$B$91</definedName>
+    <definedName name="dropped">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="261">
   <si>
     <t>id</t>
   </si>
@@ -629,9 +628,6 @@
     <t>A ratio calculated using the co-borrowers' total monthly payments on the total debt obligations, excluding mortgages and the requested LC loan, divided by the co-borrowers' combined self-reported monthly income</t>
   </si>
   <si>
-    <t>verified_status_joint</t>
-  </si>
-  <si>
     <t>Indicates if the co-borrowers' joint income was verified by LC, not verified, or if the income source was verified</t>
   </si>
   <si>
@@ -788,9 +784,6 @@
     <t>total_bc_limit</t>
   </si>
   <si>
-    <t>Attr Type</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -822,6 +815,21 @@
   </si>
   <si>
     <t>Column not in dataset</t>
+  </si>
+  <si>
+    <t>NA Values</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Constant Value</t>
+  </si>
+  <si>
+    <t>65% or more records empty</t>
+  </si>
+  <si>
+    <t>Zero Value</t>
   </si>
 </sst>
 </file>
@@ -1909,22 +1917,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="29" customWidth="1"/>
-    <col min="5" max="8" width="8.85546875" style="9"/>
-    <col min="9" max="9" width="25" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="9"/>
+    <col min="5" max="7" width="8.85546875" style="9"/>
+    <col min="8" max="8" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1935,38 +1943,38 @@
         <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -1977,24 +1985,24 @@
         <v>177</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>223</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2002,13 +2010,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2016,13 +2024,13 @@
         <v>190</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2033,10 +2041,10 @@
         <v>189</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2047,38 +2055,38 @@
         <v>153</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2089,10 +2097,10 @@
         <v>124</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2103,10 +2111,10 @@
         <v>162</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2117,10 +2125,10 @@
         <v>125</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2131,24 +2139,24 @@
         <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2162,7 +2170,7 @@
         <v>247</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2173,10 +2181,10 @@
         <v>178</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2187,10 +2195,10 @@
         <v>192</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2201,10 +2209,10 @@
         <v>185</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2215,10 +2223,10 @@
         <v>56</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2229,10 +2237,10 @@
         <v>155</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2240,13 +2248,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>247</v>
+        <v>195</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2254,13 +2262,13 @@
         <v>24</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>247</v>
+        <v>196</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2271,10 +2279,10 @@
         <v>158</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2285,10 +2293,10 @@
         <v>159</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2299,10 +2307,10 @@
         <v>57</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2313,10 +2321,10 @@
         <v>58</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2327,24 +2335,24 @@
         <v>59</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>215</v>
-      </c>
       <c r="C30" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2355,55 +2363,55 @@
         <v>60</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="B33" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>227</v>
-      </c>
       <c r="C33" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>7</v>
       </c>
@@ -2411,13 +2419,13 @@
         <v>61</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>6</v>
       </c>
@@ -2425,13 +2433,13 @@
         <v>82</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>13</v>
       </c>
@@ -2439,15 +2447,15 @@
         <v>184</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="17"/>
-    </row>
-    <row r="38" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+      <c r="H37" s="16"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>45</v>
       </c>
@@ -2455,41 +2463,41 @@
         <v>187</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>247</v>
+        <v>198</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>247</v>
+        <v>199</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
@@ -2497,13 +2505,13 @@
         <v>92</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>42</v>
       </c>
@@ -2511,13 +2519,13 @@
         <v>186</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>2</v>
       </c>
@@ -2525,13 +2533,13 @@
         <v>62</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>14</v>
       </c>
@@ -2539,25 +2547,27 @@
         <v>83</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>256</v>
+      </c>
       <c r="D45" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>1</v>
       </c>
@@ -2565,33 +2575,33 @@
         <v>63</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="I46" s="16"/>
+        <v>254</v>
+      </c>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
       <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>126</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="I47" s="16"/>
+        <v>254</v>
+      </c>
+      <c r="H47" s="16"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>118</v>
       </c>
@@ -2599,14 +2609,14 @@
         <v>127</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="I48" s="18"/>
+        <v>254</v>
+      </c>
+      <c r="H48" s="18"/>
+      <c r="I48" s="17"/>
       <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
@@ -2616,10 +2626,10 @@
         <v>128</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2630,24 +2640,24 @@
         <v>129</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2658,10 +2668,10 @@
         <v>65</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2672,10 +2682,10 @@
         <v>130</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2686,80 +2696,80 @@
         <v>66</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C55" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>240</v>
-      </c>
       <c r="C57" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.2">
@@ -2770,10 +2780,10 @@
         <v>93</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2784,10 +2794,10 @@
         <v>131</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2798,10 +2808,10 @@
         <v>136</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2812,10 +2822,10 @@
         <v>142</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2826,13 +2836,13 @@
         <v>137</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>109</v>
       </c>
@@ -2840,13 +2850,13 @@
         <v>135</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>116</v>
       </c>
@@ -2854,13 +2864,13 @@
         <v>141</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>121</v>
       </c>
@@ -2868,13 +2878,13 @@
         <v>144</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>96</v>
       </c>
@@ -2882,13 +2892,13 @@
         <v>132</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>120</v>
       </c>
@@ -2896,13 +2906,13 @@
         <v>143</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>103</v>
       </c>
@@ -2910,13 +2920,13 @@
         <v>133</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D70" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>115</v>
       </c>
@@ -2924,13 +2934,13 @@
         <v>140</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D71" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>114</v>
       </c>
@@ -2938,13 +2948,13 @@
         <v>139</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>113</v>
       </c>
@@ -2952,14 +2962,14 @@
         <v>138</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="F73" s="20"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+      <c r="E73" s="20"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>104</v>
       </c>
@@ -2967,13 +2977,13 @@
         <v>134</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D74" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>29</v>
       </c>
@@ -2981,94 +2991,94 @@
         <v>70</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B76" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="C76" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+      <c r="B79" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="B79" s="10" t="s">
-        <v>205</v>
-      </c>
       <c r="C79" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D79" s="27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B80" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="B80" s="10" t="s">
-        <v>217</v>
-      </c>
       <c r="C80" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B81" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B81" s="10" t="s">
-        <v>219</v>
-      </c>
       <c r="C81" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3079,10 +3089,10 @@
         <v>84</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D82" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -3093,10 +3103,10 @@
         <v>85</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D83" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -3107,24 +3117,24 @@
         <v>145</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B85" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -3135,10 +3145,10 @@
         <v>176</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3149,10 +3159,10 @@
         <v>72</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D87" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3163,10 +3173,10 @@
         <v>146</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D88" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,10 +3187,10 @@
         <v>175</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D89" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3191,10 +3201,10 @@
         <v>86</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D90" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3205,10 +3215,10 @@
         <v>161</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D91" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3219,10 +3229,10 @@
         <v>73</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D92" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -3233,10 +3243,10 @@
         <v>74</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D93" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3247,10 +3257,10 @@
         <v>75</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D94" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,10 +3271,10 @@
         <v>147</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D95" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3275,10 +3285,10 @@
         <v>76</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D96" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3289,10 +3299,10 @@
         <v>77</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D97" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -3303,10 +3313,10 @@
         <v>150</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D98" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -3317,10 +3327,10 @@
         <v>149</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D99" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3331,10 +3341,10 @@
         <v>148</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D100" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -3345,66 +3355,66 @@
         <v>78</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D101" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D102" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="B103" s="10" t="s">
-        <v>213</v>
-      </c>
       <c r="C103" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B104" s="10" t="s">
         <v>80</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3415,10 +3425,10 @@
         <v>151</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -3429,10 +3439,10 @@
         <v>87</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -3443,10 +3453,10 @@
         <v>88</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -3457,10 +3467,10 @@
         <v>90</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,10 +3481,10 @@
         <v>89</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -3485,24 +3495,24 @@
         <v>91</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D111" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>152</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="D112" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -3513,38 +3523,38 @@
         <v>81</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D113" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>160</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D114" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="B115" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B115" s="31" t="s">
-        <v>194</v>
-      </c>
       <c r="C115" s="32" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -3555,10 +3565,10 @@
         <v>182</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D116" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3567,746 +3577,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K116" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J116" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB589616-9200-4F38-A7CC-F0B3F4EFA91F}">
-  <dimension ref="A3:B91"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B91"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>242</v>
-      </c>
-      <c r="B4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>233</v>
-      </c>
-      <c r="B13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>234</v>
-      </c>
-      <c r="B14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>245</v>
-      </c>
-      <c r="B18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B26" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B31" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>254</v>
-      </c>
-      <c r="B32" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>220</v>
-      </c>
-      <c r="B33" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>237</v>
-      </c>
-      <c r="B37" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>204</v>
-      </c>
-      <c r="B39" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>216</v>
-      </c>
-      <c r="B40" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>239</v>
-      </c>
-      <c r="B41" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B44" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>163</v>
-      </c>
-      <c r="B46" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>228</v>
-      </c>
-      <c r="B50" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>243</v>
-      </c>
-      <c r="B51" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>45</v>
-      </c>
-      <c r="B52" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>32</v>
-      </c>
-      <c r="B53" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>232</v>
-      </c>
-      <c r="B54" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>117</v>
-      </c>
-      <c r="B55" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>212</v>
-      </c>
-      <c r="B56" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>191</v>
-      </c>
-      <c r="B58" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>208</v>
-      </c>
-      <c r="B61" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>230</v>
-      </c>
-      <c r="B63" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>218</v>
-      </c>
-      <c r="B66" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>224</v>
-      </c>
-      <c r="B68" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B69" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>112</v>
-      </c>
-      <c r="B70" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>188</v>
-      </c>
-      <c r="B72" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>40</v>
-      </c>
-      <c r="B73" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>35</v>
-      </c>
-      <c r="B74" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>210</v>
-      </c>
-      <c r="B75" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>115</v>
-      </c>
-      <c r="B76" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>114</v>
-      </c>
-      <c r="B78" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>43</v>
-      </c>
-      <c r="B79" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>120</v>
-      </c>
-      <c r="B82" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>241</v>
-      </c>
-      <c r="B83" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>26</v>
-      </c>
-      <c r="B84" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>238</v>
-      </c>
-      <c r="B85" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>17</v>
-      </c>
-      <c r="B86" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>104</v>
-      </c>
-      <c r="B87" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>244</v>
-      </c>
-      <c r="B89" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>123</v>
-      </c>
-      <c r="B90" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>16</v>
-      </c>
-      <c r="B91" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>